<commit_message>
fills out catch metadata table and starts trap metadata table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Downloads/metadata template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2086FF-D71F-7F41-B007-3B172EC4BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35540" yWindow="-20160" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -74,6 +74,127 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>sample_date</t>
+  </si>
+  <si>
+    <t>sample_time</t>
+  </si>
+  <si>
+    <t>station_code</t>
+  </si>
+  <si>
+    <t>common_name</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>fork_length</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>life_stage</t>
+  </si>
+  <si>
+    <t>r_catch</t>
+  </si>
+  <si>
+    <t>interp</t>
+  </si>
+  <si>
+    <t>brood_year</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Identifier of the sample</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Date the sample was colelcted</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>2022-10-01</t>
+  </si>
+  <si>
+    <t>2022-11-21</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>23:58:00</t>
+  </si>
+  <si>
+    <t>Time the sample was collected</t>
+  </si>
+  <si>
+    <t>Code identifying the station where the sample was collected. Levels = c("UBC", "LCC", "UCC")</t>
+  </si>
+  <si>
+    <t>Common name of the fish</t>
+  </si>
+  <si>
+    <t>Count of the fish</t>
+  </si>
+  <si>
+    <t>Fork length of the fish</t>
+  </si>
+  <si>
+    <t>Weight of the fish</t>
+  </si>
+  <si>
+    <t>Lifestage identified of the fish. Levels = c("not recorded", "fry", "yolk sac fry", "parr", "silvery parr", 
+"smolt")</t>
+  </si>
+  <si>
+    <t>Whether or not the data were interpolated. Levels = c("yes", "no")</t>
+  </si>
+  <si>
+    <t>Brood year</t>
+  </si>
+  <si>
+    <t>Run, if identified. Levels = c("not recorded", "winter", "spring", "late fall")</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>count of fish</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>gram</t>
   </si>
 </sst>
 </file>
@@ -128,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -527,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG10"/>
+  <dimension ref="A1:AMG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,26 +715,245 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10" s="6"/>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1020" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1020" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1020" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
removes some columns from trap and catch
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9AA46-2587-F94E-A2F5-35957B754788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86D753F-26BC-A34D-9CC0-102B634B81F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35540" yWindow="-20160" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="1760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -76,18 +76,6 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>sample_id</t>
-  </si>
-  <si>
-    <t>sample_date</t>
-  </si>
-  <si>
-    <t>sample_time</t>
-  </si>
-  <si>
-    <t>station_code</t>
-  </si>
-  <si>
     <t>common_name</t>
   </si>
   <si>
@@ -112,67 +100,24 @@
     <t>brood_year</t>
   </si>
   <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>Identifier of the sample</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>Date the sample was colelcted</t>
-  </si>
-  <si>
     <t>dateTime</t>
   </si>
   <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>2022-10-01</t>
-  </si>
-  <si>
-    <t>2022-11-21</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
-    <t>23:58:00</t>
-  </si>
-  <si>
-    <t>Time the sample was collected</t>
-  </si>
-  <si>
-    <t>Code identifying the station where the sample was collected. Levels = c("UBC", "LCC", "UCC")</t>
-  </si>
-  <si>
-    <t>Common name of the fish</t>
-  </si>
-  <si>
-    <t>Count of the fish</t>
-  </si>
-  <si>
     <t>Fork length of the fish</t>
   </si>
   <si>
     <t>Weight of the fish</t>
   </si>
   <si>
-    <t>Lifestage identified of the fish. Levels = c("not recorded", "fry", "yolk sac fry", "parr", "silvery parr", 
-"smolt")</t>
-  </si>
-  <si>
-    <t>Whether or not the data were interpolated. Levels = c("yes", "no")</t>
-  </si>
-  <si>
     <t>Brood year</t>
   </si>
   <si>
-    <t>Run, if identified. Levels = c("not recorded", "winter", "spring", "late fall")</t>
-  </si>
-  <si>
     <t>ratio</t>
   </si>
   <si>
@@ -194,25 +139,105 @@
     <t>ordinal</t>
   </si>
   <si>
-    <t>HH:MM:SS</t>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>fish_flts</t>
+  </si>
+  <si>
+    <t>MM-DD-YY hh:mm:ss</t>
+  </si>
+  <si>
+    <t>01/01/21 00:00:00</t>
+  </si>
+  <si>
+    <t>12/31/21 09:56:38</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>Count of fish</t>
+  </si>
+  <si>
+    <t>age_class</t>
+  </si>
+  <si>
+    <t>Age class of the fish, if identified. Levels = c("AGE0+", "", "YOY")</t>
+  </si>
+  <si>
+    <t>subsample</t>
+  </si>
+  <si>
+    <t>Levels = c("not provided", "1/4", "1/8", "1/2", "1/16", "1/32", "1/64", 
+"1/256", "")</t>
+  </si>
+  <si>
+    <t>Common name of the fish. Levels = c("Rainbow Trout", "Chinook Salmon", "Sacramento Pikeminnow", 
+"Pacific Lamprey ammocoete", "Pacific Lamprey macropthalmia", 
+"Hardhead", "Unidentified Cyprinid fry", "Sacramento Sucker", 
+"Riffle Sculpin", "Tule Perch", "Unidentified ammocoete", "Green Sunfish", 
+"Unidentified Cottus fry", "Unidentified fry", "Pumpkinseed", 
+"Threespine Stickleback", "Western Mosquitofish", "Prickly Sculpin", 
+"California Roach", "Pacific Brook Lamprey", "Sacramento Sucker fry", 
+"Speckled Dace", "Unidentified Centrarchid fry", "Black Bullhead"
+)</t>
+  </si>
+  <si>
+    <t>Lifestage of the fish. Levels = c("parr", "silvery parr", "obvious fry", "not provided", "smolt", 
+"yolk sac fry", "fry", "adult")</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>fws_race</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>2029-03-29</t>
+  </si>
+  <si>
+    <t>Date and time that the data was entered.</t>
+  </si>
+  <si>
+    <t>Catch number used to generate passage indices for reports, plus counts are split into races, zero fork lengths have been assigned</t>
+  </si>
+  <si>
+    <t>USFWS run designation base upon location or emergence timing used in reports and for passage indices. Levels = c(NA, "Winter", "Fall", "Spring", "Late-Fall", "not provided"
+)</t>
+  </si>
+  <si>
+    <t>Database generated Sheila Greene run designation of catch. Levels = c("not provided", "Winter", "Fall", "Spring", "Late-Fall", NA
+)</t>
+  </si>
+  <si>
+    <t>Whether or not the fish was dead. Levels = c(TRUE, FALSE)</t>
+  </si>
+  <si>
+    <t>Is RCatch value an interpolated catch for times the trap did not fish? . Levels = c(TRUE, FALSE)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -249,12 +274,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -262,13 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,25 +671,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG14"/>
+  <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -678,291 +699,450 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
+      <c r="B5" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>168.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>8451</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
+      <c r="B7" t="s">
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
+      <c r="B8" t="s">
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>70.2</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>30</v>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1020" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1023" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1020" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1023" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1020" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1023" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -985,19 +1165,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates catch metadata table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86D753F-26BC-A34D-9CC0-102B634B81F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B0D0EA-B12B-4C4A-AFD8-4688D8BD8373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -140,18 +140,6 @@
   </si>
   <si>
     <t>catch</t>
-  </si>
-  <si>
-    <t>fish_flts</t>
-  </si>
-  <si>
-    <t>MM-DD-YY hh:mm:ss</t>
-  </si>
-  <si>
-    <t>01/01/21 00:00:00</t>
-  </si>
-  <si>
-    <t>12/31/21 09:56:38</t>
   </si>
   <si>
     <t>dead</t>
@@ -176,27 +164,6 @@
 "1/256", "")</t>
   </si>
   <si>
-    <t>Common name of the fish. Levels = c("Rainbow Trout", "Chinook Salmon", "Sacramento Pikeminnow", 
-"Pacific Lamprey ammocoete", "Pacific Lamprey macropthalmia", 
-"Hardhead", "Unidentified Cyprinid fry", "Sacramento Sucker", 
-"Riffle Sculpin", "Tule Perch", "Unidentified ammocoete", "Green Sunfish", 
-"Unidentified Cottus fry", "Unidentified fry", "Pumpkinseed", 
-"Threespine Stickleback", "Western Mosquitofish", "Prickly Sculpin", 
-"California Roach", "Pacific Brook Lamprey", "Sacramento Sucker fry", 
-"Speckled Dace", "Unidentified Centrarchid fry", "Black Bullhead"
-)</t>
-  </si>
-  <si>
-    <t>Lifestage of the fish. Levels = c("parr", "silvery parr", "obvious fry", "not provided", "smolt", 
-"yolk sac fry", "fry", "adult")</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>fws_race</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -204,12 +171,6 @@
   </si>
   <si>
     <t>2020-07-06</t>
-  </si>
-  <si>
-    <t>2029-03-29</t>
-  </si>
-  <si>
-    <t>Date and time that the data was entered.</t>
   </si>
   <si>
     <t>Catch number used to generate passage indices for reports, plus counts are split into races, zero fork lengths have been assigned</t>
@@ -227,6 +188,30 @@
   </si>
   <si>
     <t>Is RCatch value an interpolated catch for times the trap did not fish? . Levels = c(TRUE, FALSE)</t>
+  </si>
+  <si>
+    <t>sample_row_id</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>fws_run</t>
+  </si>
+  <si>
+    <t>Common name of the fish. Levels = c("Chinook Salmon", "Hardhead", "Rainbow Trout", "Sacramento Sucker", 
+"Sacramento Pikeminnow", "Speckled Dace", "Unidentified ammocoete", 
+"Tule Perch", "Pacific Lamprey macropthalmia", "Threespine Stickleback", 
+"Pacific Lamprey ammocoete", "Unidentified Cyprinid fry", "California Roach", 
+"Riffle Sculpin", "Sacramento Sucker fry", "Golden Shiner", "Green Sunfish", 
+"Prickly Sculpin")</t>
+  </si>
+  <si>
+    <t>Lifestage of the fish. Levels = c("not provided", "parr", "silvery parr", "obvious fry", "smolt", 
+"yolk sac fry", "fry")</t>
+  </si>
+  <si>
+    <t>2023-01-05</t>
   </si>
 </sst>
 </file>
@@ -674,7 +659,7 @@
   <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,75 +723,50 @@
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1121</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="J3" s="3"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>41</v>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>37</v>
@@ -851,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <v>168.7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -859,7 +819,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -883,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="3">
-        <v>8451</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -891,31 +851,39 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -936,13 +904,13 @@
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
@@ -984,13 +952,13 @@
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -1010,11 +978,11 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
+      <c r="B12" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
@@ -1034,11 +1002,11 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>50</v>
+      <c r="B13" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>37</v>
@@ -1056,13 +1024,13 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>37</v>
@@ -1080,13 +1048,13 @@
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -1104,10 +1072,10 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
@@ -1126,27 +1094,27 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1023" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C20 C24:C1023" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1023" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E20 E24:E1023" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1023" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F20 F24:F1023" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H20 H24:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates trap metadata table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B0D0EA-B12B-4C4A-AFD8-4688D8BD8373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CE452A-50F5-C949-8C67-A7A1A2F1C3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>2023-01-05</t>
+  </si>
+  <si>
+    <t>Row ID for the sample.</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,7 +276,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +661,7 @@
   <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,6 +727,18 @@
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -755,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>221</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -811,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <v>162</v>
+        <v>168.7</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -843,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="3">
-        <v>680</v>
+        <v>8451</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -875,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="3">
-        <v>12</v>
+        <v>8451</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -978,7 +992,7 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1002,7 +1016,7 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="1" t="s">

</xml_diff>

<commit_message>
updates metadata to reflect adding sample date and station code to catch table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CE452A-50F5-C949-8C67-A7A1A2F1C3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4463366-9460-804F-857B-06544415FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -164,12 +164,6 @@
 "1/256", "")</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>2020-07-06</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
   </si>
   <si>
     <t>Is RCatch value an interpolated catch for times the trap did not fish? . Levels = c(TRUE, FALSE)</t>
-  </si>
-  <si>
-    <t>sample_row_id</t>
   </si>
   <si>
     <t>run</t>
@@ -211,10 +202,25 @@
 "yolk sac fry", "fry")</t>
   </si>
   <si>
-    <t>2023-01-05</t>
-  </si>
-  <si>
-    <t>Row ID for the sample.</t>
+    <t>station_code</t>
+  </si>
+  <si>
+    <t>sample_date</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>Code referring to the station where the sample was taken. Levels = c("UBC", "LCC", "UCC")</t>
+  </si>
+  <si>
+    <t>Date sample was taken</t>
+  </si>
+  <si>
+    <t>2023-01-02</t>
+  </si>
+  <si>
+    <t>Sample identifier linking catch to trap table</t>
   </si>
 </sst>
 </file>
@@ -658,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG16"/>
+  <dimension ref="A1:AMG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,83 +731,98 @@
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1121</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="5"/>
       <c r="J3" s="3"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1121</v>
-      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="3"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>168.7</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -813,7 +834,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>32</v>
@@ -822,18 +843,18 @@
       <c r="J5" s="3"/>
       <c r="K5" s="5"/>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="3">
-        <v>168.7</v>
+        <v>8451</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -862,45 +883,37 @@
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="3">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3">
-        <v>8451</v>
-      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>37</v>
@@ -918,13 +931,13 @@
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
@@ -942,13 +955,13 @@
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>37</v>
@@ -966,10 +979,10 @@
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -990,10 +1003,10 @@
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1014,18 +1027,18 @@
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="3"/>
@@ -1038,37 +1051,44 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -1086,49 +1106,67 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C20 C24:C1023" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C1024 C1:C21" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E20 E24:E1023" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25:E1024 E1:E21" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F20 F24:F1023" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:F1024 F1:F21" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H20 H24:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H25:H1048576 H1:H21" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates metadata and begins creation of xml file
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4463366-9460-804F-857B-06544415FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4B49B4-E423-AC45-ACDD-00C275C74979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -667,7 +667,7 @@
   <dimension ref="A1:AMG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,6 +745,9 @@
       <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
@@ -801,6 +804,9 @@
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
@@ -833,6 +839,9 @@
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>33</v>
       </c>
@@ -864,6 +873,9 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
removes sheila green run from catch table and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4B49B4-E423-AC45-ACDD-00C275C74979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E88812-DFCB-1441-8376-4A74E93CA733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -174,17 +174,10 @@
 )</t>
   </si>
   <si>
-    <t>Database generated Sheila Greene run designation of catch. Levels = c("not provided", "Winter", "Fall", "Spring", "Late-Fall", NA
-)</t>
-  </si>
-  <si>
     <t>Whether or not the fish was dead. Levels = c(TRUE, FALSE)</t>
   </si>
   <si>
     <t>Is RCatch value an interpolated catch for times the trap did not fish? . Levels = c(TRUE, FALSE)</t>
-  </si>
-  <si>
-    <t>run</t>
   </si>
   <si>
     <t>fws_run</t>
@@ -664,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG17"/>
+  <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +762,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -898,7 +891,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
@@ -994,7 +987,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1018,7 +1011,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1039,10 +1032,10 @@
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -1063,10 +1056,10 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1089,15 +1082,15 @@
         <v>45</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -1118,10 +1111,10 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
@@ -1140,45 +1133,21 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C1024 C1:C21" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C1023 C1:C20" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25:E1024 E1:E21" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E1023 E1:E20" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:F1024 F1:F21" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24:F1023 F1:F20" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H25:H1048576 H1:H21" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H24:H1048576 H1:H20" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates metadata to reflect historical data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E88812-DFCB-1441-8376-4A74E93CA733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF25807-8138-2441-92CA-29C35A2DDF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,47 +154,18 @@
     <t>age_class</t>
   </si>
   <si>
-    <t>Age class of the fish, if identified. Levels = c("AGE0+", "", "YOY")</t>
-  </si>
-  <si>
     <t>subsample</t>
   </si>
   <si>
-    <t>Levels = c("not provided", "1/4", "1/8", "1/2", "1/16", "1/32", "1/64", 
-"1/256", "")</t>
-  </si>
-  <si>
-    <t>2020-07-06</t>
-  </si>
-  <si>
     <t>Catch number used to generate passage indices for reports, plus counts are split into races, zero fork lengths have been assigned</t>
   </si>
   <si>
-    <t>USFWS run designation base upon location or emergence timing used in reports and for passage indices. Levels = c(NA, "Winter", "Fall", "Spring", "Late-Fall", "not provided"
-)</t>
-  </si>
-  <si>
-    <t>Whether or not the fish was dead. Levels = c(TRUE, FALSE)</t>
-  </si>
-  <si>
     <t>Is RCatch value an interpolated catch for times the trap did not fish? . Levels = c(TRUE, FALSE)</t>
   </si>
   <si>
     <t>fws_run</t>
   </si>
   <si>
-    <t>Common name of the fish. Levels = c("Chinook Salmon", "Hardhead", "Rainbow Trout", "Sacramento Sucker", 
-"Sacramento Pikeminnow", "Speckled Dace", "Unidentified ammocoete", 
-"Tule Perch", "Pacific Lamprey macropthalmia", "Threespine Stickleback", 
-"Pacific Lamprey ammocoete", "Unidentified Cyprinid fry", "California Roach", 
-"Riffle Sculpin", "Sacramento Sucker fry", "Golden Shiner", "Green Sunfish", 
-"Prickly Sculpin")</t>
-  </si>
-  <si>
-    <t>Lifestage of the fish. Levels = c("not provided", "parr", "silvery parr", "obvious fry", "smolt", 
-"yolk sac fry", "fry")</t>
-  </si>
-  <si>
     <t>station_code</t>
   </si>
   <si>
@@ -204,9 +175,6 @@
     <t>sample_id</t>
   </si>
   <si>
-    <t>Code referring to the station where the sample was taken. Levels = c("UBC", "LCC", "UCC")</t>
-  </si>
-  <si>
     <t>Date sample was taken</t>
   </si>
   <si>
@@ -214,6 +182,31 @@
   </si>
   <si>
     <t>Sample identifier linking catch to trap table</t>
+  </si>
+  <si>
+    <t>1998-09-01</t>
+  </si>
+  <si>
+    <t>Whether or not the fish was dead. Levels = c(FALSE, NA, TRUE)</t>
+  </si>
+  <si>
+    <t>Age class of the fish, if identified. Levels =c(NA, "AGE0+", "YOY")</t>
+  </si>
+  <si>
+    <t>Levels = c(NA, "2017", "not provided", "F", "2004", "2007", "2008", "2010", 
+"2011", "2-Jan", "8-Jan", "S", "2009", "2015", "2016", "2005", "4-Jan", "16-Jan", "Jan-32", "Jan-64", "1/256", "0.25", "0.5", "0.125", "0.0625")</t>
+  </si>
+  <si>
+    <t>Common name of the fish. Levels = c("Sacramento Sucker", "Hardhead", "Lampetra ammocoete", "Pacific Lamprey adult","Chinook Salmon", "Sacramento Pikeminnow", "Rainbow Trout", "Unidentified Cyprinid fry","Hitch", "Pacific Lamprey macropthalmia", "Black Bullhead", "California Roach","Pacific Lamprey ammocoete", "Fathead Minnow", "Tule Perch","Riffle Sculpin", "Bluegill", "Golden Shiner", "White Catfish","Smallmouth Bass", "Prickly Sculpin", "Green Sunfish", "Threespine Stickleback","Unidentified Centrarchid fry", "Western Mosquitofish", "Speckled Dace",NA, "Spotted Bass", "Unidentified Cottus fry", "Largemouth Bass","Pumpkinseed", "Centrarchid hybrid", "Brown Bullhead", "White Crappie","Unidentified Micropterus fry", "River Lamprey", "Unidentified ammocoete","Channel Catfish", "Pacific Brook Lamprey", "Brook Trout", "American Shad","Unclassified Brook Lamprey macropthalmia", "Kern Brook Lamprey ammocoete","Kern Brook Lamprey adult", "Kern Brook Lamprey macropthalmia","Unclassified Brook Lamprey adult", "Sacramento Sucker fry","Black Crappie", "Unidentified fry")</t>
+  </si>
+  <si>
+    <t>Lifestage of the fish. Levels = c("not provided", "obvious fry", "parr", "yolk sac fry", "smolt",  "silvery parr", "adult", NA, "fry")</t>
+  </si>
+  <si>
+    <t>Code referring to the station where the sample was taken. Levels = c("UBC", "LBC", "LCC", "UCC", NA, "PHB")</t>
+  </si>
+  <si>
+    <t>USFWS run designation base upon location or emergence timing used in reports and for passage indices. Levels = c(NA, "F", "W", "S", "L", "not provided")</t>
   </si>
 </sst>
 </file>
@@ -261,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -275,6 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +656,7 @@
   <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3">
-        <v>1121</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -762,7 +758,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -813,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>168.7</v>
+        <v>646.70000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -848,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="3">
-        <v>8451</v>
+        <v>84426</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -856,7 +852,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -883,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="3">
-        <v>8451</v>
+        <v>150776</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -891,7 +887,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
@@ -915,7 +911,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -958,36 +954,37 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="10" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1011,7 +1008,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1032,10 +1029,10 @@
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -1056,10 +1053,10 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1079,18 +1076,18 @@
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -1111,10 +1108,10 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
reorders columns in catch and trap tables and updates metadata. removes baileys eff column from trap table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF25807-8138-2441-92CA-29C35A2DDF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A401A3F-C77A-F340-BA07-344D0681F9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,9 +268,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +653,7 @@
   <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +674,7 @@
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1021" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,101 +715,86 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>730</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="L3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>646.70000000000005</v>
-      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -847,7 +829,7 @@
         <v>84426</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -882,36 +864,47 @@
         <v>150776</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>730</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -927,67 +920,77 @@
       <c r="I8" s="5"/>
       <c r="J8" s="3"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="3"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>646.70000000000005</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -1003,12 +1006,12 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1027,20 +1030,20 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="3"/>
@@ -1051,46 +1054,1048 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14"/>
+      <c r="BH14"/>
+      <c r="BI14"/>
+      <c r="BJ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BM14"/>
+      <c r="BN14"/>
+      <c r="BO14"/>
+      <c r="BP14"/>
+      <c r="BQ14"/>
+      <c r="BR14"/>
+      <c r="BS14"/>
+      <c r="BT14"/>
+      <c r="BU14"/>
+      <c r="BV14"/>
+      <c r="BW14"/>
+      <c r="BX14"/>
+      <c r="BY14"/>
+      <c r="BZ14"/>
+      <c r="CA14"/>
+      <c r="CB14"/>
+      <c r="CC14"/>
+      <c r="CD14"/>
+      <c r="CE14"/>
+      <c r="CF14"/>
+      <c r="CG14"/>
+      <c r="CH14"/>
+      <c r="CI14"/>
+      <c r="CJ14"/>
+      <c r="CK14"/>
+      <c r="CL14"/>
+      <c r="CM14"/>
+      <c r="CN14"/>
+      <c r="CO14"/>
+      <c r="CP14"/>
+      <c r="CQ14"/>
+      <c r="CR14"/>
+      <c r="CS14"/>
+      <c r="CT14"/>
+      <c r="CU14"/>
+      <c r="CV14"/>
+      <c r="CW14"/>
+      <c r="CX14"/>
+      <c r="CY14"/>
+      <c r="CZ14"/>
+      <c r="DA14"/>
+      <c r="DB14"/>
+      <c r="DC14"/>
+      <c r="DD14"/>
+      <c r="DE14"/>
+      <c r="DF14"/>
+      <c r="DG14"/>
+      <c r="DH14"/>
+      <c r="DI14"/>
+      <c r="DJ14"/>
+      <c r="DK14"/>
+      <c r="DL14"/>
+      <c r="DM14"/>
+      <c r="DN14"/>
+      <c r="DO14"/>
+      <c r="DP14"/>
+      <c r="DQ14"/>
+      <c r="DR14"/>
+      <c r="DS14"/>
+      <c r="DT14"/>
+      <c r="DU14"/>
+      <c r="DV14"/>
+      <c r="DW14"/>
+      <c r="DX14"/>
+      <c r="DY14"/>
+      <c r="DZ14"/>
+      <c r="EA14"/>
+      <c r="EB14"/>
+      <c r="EC14"/>
+      <c r="ED14"/>
+      <c r="EE14"/>
+      <c r="EF14"/>
+      <c r="EG14"/>
+      <c r="EH14"/>
+      <c r="EI14"/>
+      <c r="EJ14"/>
+      <c r="EK14"/>
+      <c r="EL14"/>
+      <c r="EM14"/>
+      <c r="EN14"/>
+      <c r="EO14"/>
+      <c r="EP14"/>
+      <c r="EQ14"/>
+      <c r="ER14"/>
+      <c r="ES14"/>
+      <c r="ET14"/>
+      <c r="EU14"/>
+      <c r="EV14"/>
+      <c r="EW14"/>
+      <c r="EX14"/>
+      <c r="EY14"/>
+      <c r="EZ14"/>
+      <c r="FA14"/>
+      <c r="FB14"/>
+      <c r="FC14"/>
+      <c r="FD14"/>
+      <c r="FE14"/>
+      <c r="FF14"/>
+      <c r="FG14"/>
+      <c r="FH14"/>
+      <c r="FI14"/>
+      <c r="FJ14"/>
+      <c r="FK14"/>
+      <c r="FL14"/>
+      <c r="FM14"/>
+      <c r="FN14"/>
+      <c r="FO14"/>
+      <c r="FP14"/>
+      <c r="FQ14"/>
+      <c r="FR14"/>
+      <c r="FS14"/>
+      <c r="FT14"/>
+      <c r="FU14"/>
+      <c r="FV14"/>
+      <c r="FW14"/>
+      <c r="FX14"/>
+      <c r="FY14"/>
+      <c r="FZ14"/>
+      <c r="GA14"/>
+      <c r="GB14"/>
+      <c r="GC14"/>
+      <c r="GD14"/>
+      <c r="GE14"/>
+      <c r="GF14"/>
+      <c r="GG14"/>
+      <c r="GH14"/>
+      <c r="GI14"/>
+      <c r="GJ14"/>
+      <c r="GK14"/>
+      <c r="GL14"/>
+      <c r="GM14"/>
+      <c r="GN14"/>
+      <c r="GO14"/>
+      <c r="GP14"/>
+      <c r="GQ14"/>
+      <c r="GR14"/>
+      <c r="GS14"/>
+      <c r="GT14"/>
+      <c r="GU14"/>
+      <c r="GV14"/>
+      <c r="GW14"/>
+      <c r="GX14"/>
+      <c r="GY14"/>
+      <c r="GZ14"/>
+      <c r="HA14"/>
+      <c r="HB14"/>
+      <c r="HC14"/>
+      <c r="HD14"/>
+      <c r="HE14"/>
+      <c r="HF14"/>
+      <c r="HG14"/>
+      <c r="HH14"/>
+      <c r="HI14"/>
+      <c r="HJ14"/>
+      <c r="HK14"/>
+      <c r="HL14"/>
+      <c r="HM14"/>
+      <c r="HN14"/>
+      <c r="HO14"/>
+      <c r="HP14"/>
+      <c r="HQ14"/>
+      <c r="HR14"/>
+      <c r="HS14"/>
+      <c r="HT14"/>
+      <c r="HU14"/>
+      <c r="HV14"/>
+      <c r="HW14"/>
+      <c r="HX14"/>
+      <c r="HY14"/>
+      <c r="HZ14"/>
+      <c r="IA14"/>
+      <c r="IB14"/>
+      <c r="IC14"/>
+      <c r="ID14"/>
+      <c r="IE14"/>
+      <c r="IF14"/>
+      <c r="IG14"/>
+      <c r="IH14"/>
+      <c r="II14"/>
+      <c r="IJ14"/>
+      <c r="IK14"/>
+      <c r="IL14"/>
+      <c r="IM14"/>
+      <c r="IN14"/>
+      <c r="IO14"/>
+      <c r="IP14"/>
+      <c r="IQ14"/>
+      <c r="IR14"/>
+      <c r="IS14"/>
+      <c r="IT14"/>
+      <c r="IU14"/>
+      <c r="IV14"/>
+      <c r="IW14"/>
+      <c r="IX14"/>
+      <c r="IY14"/>
+      <c r="IZ14"/>
+      <c r="JA14"/>
+      <c r="JB14"/>
+      <c r="JC14"/>
+      <c r="JD14"/>
+      <c r="JE14"/>
+      <c r="JF14"/>
+      <c r="JG14"/>
+      <c r="JH14"/>
+      <c r="JI14"/>
+      <c r="JJ14"/>
+      <c r="JK14"/>
+      <c r="JL14"/>
+      <c r="JM14"/>
+      <c r="JN14"/>
+      <c r="JO14"/>
+      <c r="JP14"/>
+      <c r="JQ14"/>
+      <c r="JR14"/>
+      <c r="JS14"/>
+      <c r="JT14"/>
+      <c r="JU14"/>
+      <c r="JV14"/>
+      <c r="JW14"/>
+      <c r="JX14"/>
+      <c r="JY14"/>
+      <c r="JZ14"/>
+      <c r="KA14"/>
+      <c r="KB14"/>
+      <c r="KC14"/>
+      <c r="KD14"/>
+      <c r="KE14"/>
+      <c r="KF14"/>
+      <c r="KG14"/>
+      <c r="KH14"/>
+      <c r="KI14"/>
+      <c r="KJ14"/>
+      <c r="KK14"/>
+      <c r="KL14"/>
+      <c r="KM14"/>
+      <c r="KN14"/>
+      <c r="KO14"/>
+      <c r="KP14"/>
+      <c r="KQ14"/>
+      <c r="KR14"/>
+      <c r="KS14"/>
+      <c r="KT14"/>
+      <c r="KU14"/>
+      <c r="KV14"/>
+      <c r="KW14"/>
+      <c r="KX14"/>
+      <c r="KY14"/>
+      <c r="KZ14"/>
+      <c r="LA14"/>
+      <c r="LB14"/>
+      <c r="LC14"/>
+      <c r="LD14"/>
+      <c r="LE14"/>
+      <c r="LF14"/>
+      <c r="LG14"/>
+      <c r="LH14"/>
+      <c r="LI14"/>
+      <c r="LJ14"/>
+      <c r="LK14"/>
+      <c r="LL14"/>
+      <c r="LM14"/>
+      <c r="LN14"/>
+      <c r="LO14"/>
+      <c r="LP14"/>
+      <c r="LQ14"/>
+      <c r="LR14"/>
+      <c r="LS14"/>
+      <c r="LT14"/>
+      <c r="LU14"/>
+      <c r="LV14"/>
+      <c r="LW14"/>
+      <c r="LX14"/>
+      <c r="LY14"/>
+      <c r="LZ14"/>
+      <c r="MA14"/>
+      <c r="MB14"/>
+      <c r="MC14"/>
+      <c r="MD14"/>
+      <c r="ME14"/>
+      <c r="MF14"/>
+      <c r="MG14"/>
+      <c r="MH14"/>
+      <c r="MI14"/>
+      <c r="MJ14"/>
+      <c r="MK14"/>
+      <c r="ML14"/>
+      <c r="MM14"/>
+      <c r="MN14"/>
+      <c r="MO14"/>
+      <c r="MP14"/>
+      <c r="MQ14"/>
+      <c r="MR14"/>
+      <c r="MS14"/>
+      <c r="MT14"/>
+      <c r="MU14"/>
+      <c r="MV14"/>
+      <c r="MW14"/>
+      <c r="MX14"/>
+      <c r="MY14"/>
+      <c r="MZ14"/>
+      <c r="NA14"/>
+      <c r="NB14"/>
+      <c r="NC14"/>
+      <c r="ND14"/>
+      <c r="NE14"/>
+      <c r="NF14"/>
+      <c r="NG14"/>
+      <c r="NH14"/>
+      <c r="NI14"/>
+      <c r="NJ14"/>
+      <c r="NK14"/>
+      <c r="NL14"/>
+      <c r="NM14"/>
+      <c r="NN14"/>
+      <c r="NO14"/>
+      <c r="NP14"/>
+      <c r="NQ14"/>
+      <c r="NR14"/>
+      <c r="NS14"/>
+      <c r="NT14"/>
+      <c r="NU14"/>
+      <c r="NV14"/>
+      <c r="NW14"/>
+      <c r="NX14"/>
+      <c r="NY14"/>
+      <c r="NZ14"/>
+      <c r="OA14"/>
+      <c r="OB14"/>
+      <c r="OC14"/>
+      <c r="OD14"/>
+      <c r="OE14"/>
+      <c r="OF14"/>
+      <c r="OG14"/>
+      <c r="OH14"/>
+      <c r="OI14"/>
+      <c r="OJ14"/>
+      <c r="OK14"/>
+      <c r="OL14"/>
+      <c r="OM14"/>
+      <c r="ON14"/>
+      <c r="OO14"/>
+      <c r="OP14"/>
+      <c r="OQ14"/>
+      <c r="OR14"/>
+      <c r="OS14"/>
+      <c r="OT14"/>
+      <c r="OU14"/>
+      <c r="OV14"/>
+      <c r="OW14"/>
+      <c r="OX14"/>
+      <c r="OY14"/>
+      <c r="OZ14"/>
+      <c r="PA14"/>
+      <c r="PB14"/>
+      <c r="PC14"/>
+      <c r="PD14"/>
+      <c r="PE14"/>
+      <c r="PF14"/>
+      <c r="PG14"/>
+      <c r="PH14"/>
+      <c r="PI14"/>
+      <c r="PJ14"/>
+      <c r="PK14"/>
+      <c r="PL14"/>
+      <c r="PM14"/>
+      <c r="PN14"/>
+      <c r="PO14"/>
+      <c r="PP14"/>
+      <c r="PQ14"/>
+      <c r="PR14"/>
+      <c r="PS14"/>
+      <c r="PT14"/>
+      <c r="PU14"/>
+      <c r="PV14"/>
+      <c r="PW14"/>
+      <c r="PX14"/>
+      <c r="PY14"/>
+      <c r="PZ14"/>
+      <c r="QA14"/>
+      <c r="QB14"/>
+      <c r="QC14"/>
+      <c r="QD14"/>
+      <c r="QE14"/>
+      <c r="QF14"/>
+      <c r="QG14"/>
+      <c r="QH14"/>
+      <c r="QI14"/>
+      <c r="QJ14"/>
+      <c r="QK14"/>
+      <c r="QL14"/>
+      <c r="QM14"/>
+      <c r="QN14"/>
+      <c r="QO14"/>
+      <c r="QP14"/>
+      <c r="QQ14"/>
+      <c r="QR14"/>
+      <c r="QS14"/>
+      <c r="QT14"/>
+      <c r="QU14"/>
+      <c r="QV14"/>
+      <c r="QW14"/>
+      <c r="QX14"/>
+      <c r="QY14"/>
+      <c r="QZ14"/>
+      <c r="RA14"/>
+      <c r="RB14"/>
+      <c r="RC14"/>
+      <c r="RD14"/>
+      <c r="RE14"/>
+      <c r="RF14"/>
+      <c r="RG14"/>
+      <c r="RH14"/>
+      <c r="RI14"/>
+      <c r="RJ14"/>
+      <c r="RK14"/>
+      <c r="RL14"/>
+      <c r="RM14"/>
+      <c r="RN14"/>
+      <c r="RO14"/>
+      <c r="RP14"/>
+      <c r="RQ14"/>
+      <c r="RR14"/>
+      <c r="RS14"/>
+      <c r="RT14"/>
+      <c r="RU14"/>
+      <c r="RV14"/>
+      <c r="RW14"/>
+      <c r="RX14"/>
+      <c r="RY14"/>
+      <c r="RZ14"/>
+      <c r="SA14"/>
+      <c r="SB14"/>
+      <c r="SC14"/>
+      <c r="SD14"/>
+      <c r="SE14"/>
+      <c r="SF14"/>
+      <c r="SG14"/>
+      <c r="SH14"/>
+      <c r="SI14"/>
+      <c r="SJ14"/>
+      <c r="SK14"/>
+      <c r="SL14"/>
+      <c r="SM14"/>
+      <c r="SN14"/>
+      <c r="SO14"/>
+      <c r="SP14"/>
+      <c r="SQ14"/>
+      <c r="SR14"/>
+      <c r="SS14"/>
+      <c r="ST14"/>
+      <c r="SU14"/>
+      <c r="SV14"/>
+      <c r="SW14"/>
+      <c r="SX14"/>
+      <c r="SY14"/>
+      <c r="SZ14"/>
+      <c r="TA14"/>
+      <c r="TB14"/>
+      <c r="TC14"/>
+      <c r="TD14"/>
+      <c r="TE14"/>
+      <c r="TF14"/>
+      <c r="TG14"/>
+      <c r="TH14"/>
+      <c r="TI14"/>
+      <c r="TJ14"/>
+      <c r="TK14"/>
+      <c r="TL14"/>
+      <c r="TM14"/>
+      <c r="TN14"/>
+      <c r="TO14"/>
+      <c r="TP14"/>
+      <c r="TQ14"/>
+      <c r="TR14"/>
+      <c r="TS14"/>
+      <c r="TT14"/>
+      <c r="TU14"/>
+      <c r="TV14"/>
+      <c r="TW14"/>
+      <c r="TX14"/>
+      <c r="TY14"/>
+      <c r="TZ14"/>
+      <c r="UA14"/>
+      <c r="UB14"/>
+      <c r="UC14"/>
+      <c r="UD14"/>
+      <c r="UE14"/>
+      <c r="UF14"/>
+      <c r="UG14"/>
+      <c r="UH14"/>
+      <c r="UI14"/>
+      <c r="UJ14"/>
+      <c r="UK14"/>
+      <c r="UL14"/>
+      <c r="UM14"/>
+      <c r="UN14"/>
+      <c r="UO14"/>
+      <c r="UP14"/>
+      <c r="UQ14"/>
+      <c r="UR14"/>
+      <c r="US14"/>
+      <c r="UT14"/>
+      <c r="UU14"/>
+      <c r="UV14"/>
+      <c r="UW14"/>
+      <c r="UX14"/>
+      <c r="UY14"/>
+      <c r="UZ14"/>
+      <c r="VA14"/>
+      <c r="VB14"/>
+      <c r="VC14"/>
+      <c r="VD14"/>
+      <c r="VE14"/>
+      <c r="VF14"/>
+      <c r="VG14"/>
+      <c r="VH14"/>
+      <c r="VI14"/>
+      <c r="VJ14"/>
+      <c r="VK14"/>
+      <c r="VL14"/>
+      <c r="VM14"/>
+      <c r="VN14"/>
+      <c r="VO14"/>
+      <c r="VP14"/>
+      <c r="VQ14"/>
+      <c r="VR14"/>
+      <c r="VS14"/>
+      <c r="VT14"/>
+      <c r="VU14"/>
+      <c r="VV14"/>
+      <c r="VW14"/>
+      <c r="VX14"/>
+      <c r="VY14"/>
+      <c r="VZ14"/>
+      <c r="WA14"/>
+      <c r="WB14"/>
+      <c r="WC14"/>
+      <c r="WD14"/>
+      <c r="WE14"/>
+      <c r="WF14"/>
+      <c r="WG14"/>
+      <c r="WH14"/>
+      <c r="WI14"/>
+      <c r="WJ14"/>
+      <c r="WK14"/>
+      <c r="WL14"/>
+      <c r="WM14"/>
+      <c r="WN14"/>
+      <c r="WO14"/>
+      <c r="WP14"/>
+      <c r="WQ14"/>
+      <c r="WR14"/>
+      <c r="WS14"/>
+      <c r="WT14"/>
+      <c r="WU14"/>
+      <c r="WV14"/>
+      <c r="WW14"/>
+      <c r="WX14"/>
+      <c r="WY14"/>
+      <c r="WZ14"/>
+      <c r="XA14"/>
+      <c r="XB14"/>
+      <c r="XC14"/>
+      <c r="XD14"/>
+      <c r="XE14"/>
+      <c r="XF14"/>
+      <c r="XG14"/>
+      <c r="XH14"/>
+      <c r="XI14"/>
+      <c r="XJ14"/>
+      <c r="XK14"/>
+      <c r="XL14"/>
+      <c r="XM14"/>
+      <c r="XN14"/>
+      <c r="XO14"/>
+      <c r="XP14"/>
+      <c r="XQ14"/>
+      <c r="XR14"/>
+      <c r="XS14"/>
+      <c r="XT14"/>
+      <c r="XU14"/>
+      <c r="XV14"/>
+      <c r="XW14"/>
+      <c r="XX14"/>
+      <c r="XY14"/>
+      <c r="XZ14"/>
+      <c r="YA14"/>
+      <c r="YB14"/>
+      <c r="YC14"/>
+      <c r="YD14"/>
+      <c r="YE14"/>
+      <c r="YF14"/>
+      <c r="YG14"/>
+      <c r="YH14"/>
+      <c r="YI14"/>
+      <c r="YJ14"/>
+      <c r="YK14"/>
+      <c r="YL14"/>
+      <c r="YM14"/>
+      <c r="YN14"/>
+      <c r="YO14"/>
+      <c r="YP14"/>
+      <c r="YQ14"/>
+      <c r="YR14"/>
+      <c r="YS14"/>
+      <c r="YT14"/>
+      <c r="YU14"/>
+      <c r="YV14"/>
+      <c r="YW14"/>
+      <c r="YX14"/>
+      <c r="YY14"/>
+      <c r="YZ14"/>
+      <c r="ZA14"/>
+      <c r="ZB14"/>
+      <c r="ZC14"/>
+      <c r="ZD14"/>
+      <c r="ZE14"/>
+      <c r="ZF14"/>
+      <c r="ZG14"/>
+      <c r="ZH14"/>
+      <c r="ZI14"/>
+      <c r="ZJ14"/>
+      <c r="ZK14"/>
+      <c r="ZL14"/>
+      <c r="ZM14"/>
+      <c r="ZN14"/>
+      <c r="ZO14"/>
+      <c r="ZP14"/>
+      <c r="ZQ14"/>
+      <c r="ZR14"/>
+      <c r="ZS14"/>
+      <c r="ZT14"/>
+      <c r="ZU14"/>
+      <c r="ZV14"/>
+      <c r="ZW14"/>
+      <c r="ZX14"/>
+      <c r="ZY14"/>
+      <c r="ZZ14"/>
+      <c r="AAA14"/>
+      <c r="AAB14"/>
+      <c r="AAC14"/>
+      <c r="AAD14"/>
+      <c r="AAE14"/>
+      <c r="AAF14"/>
+      <c r="AAG14"/>
+      <c r="AAH14"/>
+      <c r="AAI14"/>
+      <c r="AAJ14"/>
+      <c r="AAK14"/>
+      <c r="AAL14"/>
+      <c r="AAM14"/>
+      <c r="AAN14"/>
+      <c r="AAO14"/>
+      <c r="AAP14"/>
+      <c r="AAQ14"/>
+      <c r="AAR14"/>
+      <c r="AAS14"/>
+      <c r="AAT14"/>
+      <c r="AAU14"/>
+      <c r="AAV14"/>
+      <c r="AAW14"/>
+      <c r="AAX14"/>
+      <c r="AAY14"/>
+      <c r="AAZ14"/>
+      <c r="ABA14"/>
+      <c r="ABB14"/>
+      <c r="ABC14"/>
+      <c r="ABD14"/>
+      <c r="ABE14"/>
+      <c r="ABF14"/>
+      <c r="ABG14"/>
+      <c r="ABH14"/>
+      <c r="ABI14"/>
+      <c r="ABJ14"/>
+      <c r="ABK14"/>
+      <c r="ABL14"/>
+      <c r="ABM14"/>
+      <c r="ABN14"/>
+      <c r="ABO14"/>
+      <c r="ABP14"/>
+      <c r="ABQ14"/>
+      <c r="ABR14"/>
+      <c r="ABS14"/>
+      <c r="ABT14"/>
+      <c r="ABU14"/>
+      <c r="ABV14"/>
+      <c r="ABW14"/>
+      <c r="ABX14"/>
+      <c r="ABY14"/>
+      <c r="ABZ14"/>
+      <c r="ACA14"/>
+      <c r="ACB14"/>
+      <c r="ACC14"/>
+      <c r="ACD14"/>
+      <c r="ACE14"/>
+      <c r="ACF14"/>
+      <c r="ACG14"/>
+      <c r="ACH14"/>
+      <c r="ACI14"/>
+      <c r="ACJ14"/>
+      <c r="ACK14"/>
+      <c r="ACL14"/>
+      <c r="ACM14"/>
+      <c r="ACN14"/>
+      <c r="ACO14"/>
+      <c r="ACP14"/>
+      <c r="ACQ14"/>
+      <c r="ACR14"/>
+      <c r="ACS14"/>
+      <c r="ACT14"/>
+      <c r="ACU14"/>
+      <c r="ACV14"/>
+      <c r="ACW14"/>
+      <c r="ACX14"/>
+      <c r="ACY14"/>
+      <c r="ACZ14"/>
+      <c r="ADA14"/>
+      <c r="ADB14"/>
+      <c r="ADC14"/>
+      <c r="ADD14"/>
+      <c r="ADE14"/>
+      <c r="ADF14"/>
+      <c r="ADG14"/>
+      <c r="ADH14"/>
+      <c r="ADI14"/>
+      <c r="ADJ14"/>
+      <c r="ADK14"/>
+      <c r="ADL14"/>
+      <c r="ADM14"/>
+      <c r="ADN14"/>
+      <c r="ADO14"/>
+      <c r="ADP14"/>
+      <c r="ADQ14"/>
+      <c r="ADR14"/>
+      <c r="ADS14"/>
+      <c r="ADT14"/>
+      <c r="ADU14"/>
+      <c r="ADV14"/>
+      <c r="ADW14"/>
+      <c r="ADX14"/>
+      <c r="ADY14"/>
+      <c r="ADZ14"/>
+      <c r="AEA14"/>
+      <c r="AEB14"/>
+      <c r="AEC14"/>
+      <c r="AED14"/>
+      <c r="AEE14"/>
+      <c r="AEF14"/>
+      <c r="AEG14"/>
+      <c r="AEH14"/>
+      <c r="AEI14"/>
+      <c r="AEJ14"/>
+      <c r="AEK14"/>
+      <c r="AEL14"/>
+      <c r="AEM14"/>
+      <c r="AEN14"/>
+      <c r="AEO14"/>
+      <c r="AEP14"/>
+      <c r="AEQ14"/>
+      <c r="AER14"/>
+      <c r="AES14"/>
+      <c r="AET14"/>
+      <c r="AEU14"/>
+      <c r="AEV14"/>
+      <c r="AEW14"/>
+      <c r="AEX14"/>
+      <c r="AEY14"/>
+      <c r="AEZ14"/>
+      <c r="AFA14"/>
+      <c r="AFB14"/>
+      <c r="AFC14"/>
+      <c r="AFD14"/>
+      <c r="AFE14"/>
+      <c r="AFF14"/>
+      <c r="AFG14"/>
+      <c r="AFH14"/>
+      <c r="AFI14"/>
+      <c r="AFJ14"/>
+      <c r="AFK14"/>
+      <c r="AFL14"/>
+      <c r="AFM14"/>
+      <c r="AFN14"/>
+      <c r="AFO14"/>
+      <c r="AFP14"/>
+      <c r="AFQ14"/>
+      <c r="AFR14"/>
+      <c r="AFS14"/>
+      <c r="AFT14"/>
+      <c r="AFU14"/>
+      <c r="AFV14"/>
+      <c r="AFW14"/>
+      <c r="AFX14"/>
+      <c r="AFY14"/>
+      <c r="AFZ14"/>
+      <c r="AGA14"/>
+      <c r="AGB14"/>
+      <c r="AGC14"/>
+      <c r="AGD14"/>
+      <c r="AGE14"/>
+      <c r="AGF14"/>
+      <c r="AGG14"/>
+      <c r="AGH14"/>
+      <c r="AGI14"/>
+      <c r="AGJ14"/>
+      <c r="AGK14"/>
+      <c r="AGL14"/>
+      <c r="AGM14"/>
+      <c r="AGN14"/>
+      <c r="AGO14"/>
+      <c r="AGP14"/>
+      <c r="AGQ14"/>
+      <c r="AGR14"/>
+      <c r="AGS14"/>
+      <c r="AGT14"/>
+      <c r="AGU14"/>
+      <c r="AGV14"/>
+      <c r="AGW14"/>
+      <c r="AGX14"/>
+      <c r="AGY14"/>
+      <c r="AGZ14"/>
+      <c r="AHA14"/>
+      <c r="AHB14"/>
+      <c r="AHC14"/>
+      <c r="AHD14"/>
+      <c r="AHE14"/>
+      <c r="AHF14"/>
+      <c r="AHG14"/>
+      <c r="AHH14"/>
+      <c r="AHI14"/>
+      <c r="AHJ14"/>
+      <c r="AHK14"/>
+      <c r="AHL14"/>
+      <c r="AHM14"/>
+      <c r="AHN14"/>
+      <c r="AHO14"/>
+      <c r="AHP14"/>
+      <c r="AHQ14"/>
+      <c r="AHR14"/>
+      <c r="AHS14"/>
+      <c r="AHT14"/>
+      <c r="AHU14"/>
+      <c r="AHV14"/>
+      <c r="AHW14"/>
+      <c r="AHX14"/>
+      <c r="AHY14"/>
+      <c r="AHZ14"/>
+      <c r="AIA14"/>
+      <c r="AIB14"/>
+      <c r="AIC14"/>
+      <c r="AID14"/>
+      <c r="AIE14"/>
+      <c r="AIF14"/>
+      <c r="AIG14"/>
+      <c r="AIH14"/>
+      <c r="AII14"/>
+      <c r="AIJ14"/>
+      <c r="AIK14"/>
+      <c r="AIL14"/>
+      <c r="AIM14"/>
+      <c r="AIN14"/>
+      <c r="AIO14"/>
+      <c r="AIP14"/>
+      <c r="AIQ14"/>
+      <c r="AIR14"/>
+      <c r="AIS14"/>
+      <c r="AIT14"/>
+      <c r="AIU14"/>
+      <c r="AIV14"/>
+      <c r="AIW14"/>
+      <c r="AIX14"/>
+      <c r="AIY14"/>
+      <c r="AIZ14"/>
+      <c r="AJA14"/>
+      <c r="AJB14"/>
+      <c r="AJC14"/>
+      <c r="AJD14"/>
+      <c r="AJE14"/>
+      <c r="AJF14"/>
+      <c r="AJG14"/>
+      <c r="AJH14"/>
+      <c r="AJI14"/>
+      <c r="AJJ14"/>
+      <c r="AJK14"/>
+      <c r="AJL14"/>
+      <c r="AJM14"/>
+      <c r="AJN14"/>
+      <c r="AJO14"/>
+      <c r="AJP14"/>
+      <c r="AJQ14"/>
+      <c r="AJR14"/>
+      <c r="AJS14"/>
+      <c r="AJT14"/>
+      <c r="AJU14"/>
+      <c r="AJV14"/>
+      <c r="AJW14"/>
+      <c r="AJX14"/>
+      <c r="AJY14"/>
+      <c r="AJZ14"/>
+      <c r="AKA14"/>
+      <c r="AKB14"/>
+      <c r="AKC14"/>
+      <c r="AKD14"/>
+      <c r="AKE14"/>
+      <c r="AKF14"/>
+      <c r="AKG14"/>
+      <c r="AKH14"/>
+      <c r="AKI14"/>
+      <c r="AKJ14"/>
+      <c r="AKK14"/>
+      <c r="AKL14"/>
+      <c r="AKM14"/>
+      <c r="AKN14"/>
+      <c r="AKO14"/>
+      <c r="AKP14"/>
+      <c r="AKQ14"/>
+      <c r="AKR14"/>
+      <c r="AKS14"/>
+      <c r="AKT14"/>
+      <c r="AKU14"/>
+      <c r="AKV14"/>
+      <c r="AKW14"/>
+      <c r="AKX14"/>
+      <c r="AKY14"/>
+      <c r="AKZ14"/>
+      <c r="ALA14"/>
+      <c r="ALB14"/>
+      <c r="ALC14"/>
+      <c r="ALD14"/>
+      <c r="ALE14"/>
+      <c r="ALF14"/>
+      <c r="ALG14"/>
+      <c r="ALH14"/>
+      <c r="ALI14"/>
+      <c r="ALJ14"/>
+      <c r="ALK14"/>
+      <c r="ALL14"/>
+      <c r="ALM14"/>
+      <c r="ALN14"/>
+      <c r="ALO14"/>
+      <c r="ALP14"/>
+      <c r="ALQ14"/>
+      <c r="ALR14"/>
+      <c r="ALS14"/>
+      <c r="ALT14"/>
+      <c r="ALU14"/>
+      <c r="ALV14"/>
+      <c r="ALW14"/>
+      <c r="ALX14"/>
+      <c r="ALY14"/>
+      <c r="ALZ14"/>
+      <c r="AMA14"/>
+      <c r="AMB14"/>
+      <c r="AMC14"/>
+      <c r="AMD14"/>
+      <c r="AME14"/>
+      <c r="AMF14"/>
+      <c r="AMG14"/>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -1106,12 +2111,12 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1021" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
@@ -1132,19 +2137,19 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C1023 C1:C20" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C1023 C1:C16 C17:C20" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E1023 E1:E20" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E1023 E1:E16 E17:E20" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24:F1023 F1:F20" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24:F1023 F1:F16 F17:F20" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H24:H1048576 H1:H20" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H24:H1048576 H1:H16 H17:H20" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates levels for fws_run in catch to be more specific
</commit_message>
<xml_diff>
--- a/data-raw/metadata/catch-metadata.xlsx
+++ b/data-raw/metadata/catch-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A401A3F-C77A-F340-BA07-344D0681F9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4F136-468C-9348-9D6A-9D6508670C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,7 +206,7 @@
     <t>Code referring to the station where the sample was taken. Levels = c("UBC", "LBC", "LCC", "UCC", NA, "PHB")</t>
   </si>
   <si>
-    <t>USFWS run designation base upon location or emergence timing used in reports and for passage indices. Levels = c(NA, "F", "W", "S", "L", "not provided")</t>
+    <t>USFWS run designation base upon location or emergence timing used in reports and for passage indices. Levels = c(NA, "fall", "winter", "spring", "late-fall")</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:AMG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>